<commit_message>
Restore formula for R&D S-curve in Supporting Calculations (#204)
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/FoPITY/Supporting Calculations for Policy Schedules.xlsx
+++ b/InputData/plcy-schd/FoPITY/Supporting Calculations for Policy Schedules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\plcy-schd\FoPITY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2265921B-CE1B-4A16-8B99-4213997FFE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7300916-EA8E-48F2-A9A1-CEF97C48C667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18165" yWindow="0" windowWidth="27855" windowHeight="21855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10515" yWindow="240" windowWidth="27855" windowHeight="21855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -3161,90 +3161,119 @@
         <v>0</v>
       </c>
       <c r="C47">
+        <f t="shared" ref="C47:U47" si="0">$B$15/(1+EXP($B$16*(B46-$B46+$B$17)))</f>
         <v>1.1317442005127826E-2</v>
       </c>
       <c r="D47">
+        <f t="shared" si="0"/>
         <v>1.5068964918956498E-2</v>
       </c>
       <c r="E47">
+        <f t="shared" si="0"/>
         <v>2.0039464446169435E-2</v>
       </c>
       <c r="F47">
+        <f t="shared" si="0"/>
         <v>2.6606291127741783E-2</v>
       </c>
       <c r="G47">
+        <f t="shared" si="0"/>
         <v>3.5249552635410054E-2</v>
       </c>
       <c r="H47">
+        <f t="shared" si="0"/>
         <v>4.6569675006453516E-2</v>
       </c>
       <c r="I47">
+        <f t="shared" si="0"/>
         <v>6.1300011521898706E-2</v>
       </c>
       <c r="J47">
+        <f t="shared" si="0"/>
         <v>8.0307238087136135E-2</v>
       </c>
       <c r="K47">
+        <f t="shared" si="0"/>
         <v>0.10456852091885868</v>
       </c>
       <c r="L47">
+        <f t="shared" si="0"/>
         <v>0.13511100856602506</v>
       </c>
       <c r="M47">
+        <f t="shared" si="0"/>
         <v>0.172898634257765</v>
       </c>
       <c r="N47">
+        <f t="shared" si="0"/>
         <v>0.21865784601125693</v>
       </c>
       <c r="O47">
+        <f t="shared" si="0"/>
         <v>0.27265254556539109</v>
       </c>
       <c r="P47">
+        <f t="shared" si="0"/>
         <v>0.33445022305911554</v>
       </c>
       <c r="Q47">
+        <f t="shared" si="0"/>
         <v>0.40275633722650384</v>
       </c>
       <c r="R47">
+        <f t="shared" si="0"/>
         <v>0.47540871426241038</v>
       </c>
       <c r="S47">
+        <f t="shared" si="0"/>
         <v>0.54959128573758953</v>
       </c>
       <c r="T47">
+        <f t="shared" si="0"/>
         <v>0.62224366277349608</v>
       </c>
       <c r="U47">
+        <f t="shared" si="0"/>
         <v>0.69054977694088449</v>
       </c>
       <c r="V47">
+        <f>$B$15/(1+EXP($B$16*(U46-$B46+$B$17)))</f>
         <v>0.75234745443460882</v>
       </c>
       <c r="W47">
+        <f t="shared" ref="W47" si="1">$B$15/(1+EXP($B$16*(V46-$B46+$B$17)))</f>
         <v>0.80634215398874309</v>
       </c>
       <c r="X47">
+        <f t="shared" ref="X47" si="2">$B$15/(1+EXP($B$16*(W46-$B46+$B$17)))</f>
         <v>0.85210136574223494</v>
       </c>
       <c r="Y47">
+        <f>$B$15/(1+EXP($B$16*(X46-$B46+$B$17)))</f>
         <v>0.88988899143397482</v>
       </c>
       <c r="Z47">
+        <f t="shared" ref="Z47" si="3">$B$15/(1+EXP($B$16*(Y46-$B46+$B$17)))</f>
         <v>0.9204314790811412</v>
       </c>
       <c r="AA47">
+        <f t="shared" ref="AA47" si="4">$B$15/(1+EXP($B$16*(Z46-$B46+$B$17)))</f>
         <v>0.94469276191286389</v>
       </c>
       <c r="AB47">
+        <f t="shared" ref="AB47" si="5">$B$15/(1+EXP($B$16*(AA46-$B46+$B$17)))</f>
         <v>0.96369998847810123</v>
       </c>
       <c r="AC47">
+        <f t="shared" ref="AC47" si="6">$B$15/(1+EXP($B$16*(AB46-$B46+$B$17)))</f>
         <v>0.97843032499354643</v>
       </c>
       <c r="AD47">
+        <f t="shared" ref="AD47" si="7">$B$15/(1+EXP($B$16*(AC46-$B46+$B$17)))</f>
         <v>0.98975044736458984</v>
       </c>
       <c r="AE47">
+        <f t="shared" ref="AE47" si="8">$B$15/(1+EXP($B$16*(AD46-$B46+$B$17)))</f>
         <v>0.99839370887225809</v>
       </c>
     </row>

</xml_diff>